<commit_message>
Updated PPT, Domain, and Storyboards
</commit_message>
<xml_diff>
--- a/Project Documents/Story Boards/Kitchen Display.xlsx
+++ b/Project Documents/Story Boards/Kitchen Display.xlsx
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Order Number</t>
   </si>
@@ -52,6 +53,21 @@
   </si>
   <si>
     <t>Ranch Dressing</t>
+  </si>
+  <si>
+    <t>Elapsed Time (min)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Frank</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Charlie</t>
   </si>
 </sst>
 </file>
@@ -87,13 +103,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -104,11 +130,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F1048576" totalsRowShown="0">
-  <autoFilter ref="A1:F1048576"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G1048576" totalsRowShown="0">
+  <autoFilter ref="A1:G1048576"/>
+  <tableColumns count="7">
     <tableColumn id="1" name="Order Number"/>
-    <tableColumn id="2" name="Prep Time (Mins)"/>
+    <tableColumn id="2" name="Prep Time (Mins)" dataDxfId="1"/>
+    <tableColumn id="7" name="Elapsed Time (min)" dataDxfId="0"/>
     <tableColumn id="3" name="Dish"/>
     <tableColumn id="4" name="Notes"/>
     <tableColumn id="5" name="Assigned to"/>
@@ -405,90 +432,118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>911</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>30</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>911</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
       </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>912</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>30</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
         <v>9</v>
       </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>912</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>